<commit_message>
Separacion de metodos. Agregado menu, mostarRegistros, agregarRegistros
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ficheros-Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MG\grupo8\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr documentId="13_ncr:1_{ECAA8EFA-2317-4DFA-9F6B-58F3A422B155}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView windowHeight="8625" windowWidth="12210" xWindow="0" yWindow="0"/>
+    <workbookView windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="Java Books" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
   <si>
     <t>No</t>
   </si>
@@ -96,12 +98,51 @@
   </si>
   <si>
     <t>Jez Humble</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>El que se duerme pierde</t>
+  </si>
+  <si>
+    <t>Tom Peter</t>
+  </si>
+  <si>
+    <t>Sin lugar a duda</t>
+  </si>
+  <si>
+    <t>Ana Gutierrez</t>
+  </si>
+  <si>
+    <t>El arte de dormir</t>
+  </si>
+  <si>
+    <t>Nico</t>
+  </si>
+  <si>
+    <t>Buscando a Nemo</t>
+  </si>
+  <si>
+    <t>Humble Po</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -413,20 +454,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.28515625" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.28515625" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.33203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,7 +481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -454,7 +495,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -468,7 +509,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -482,7 +523,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -496,7 +537,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -510,7 +551,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -524,9 +565,9 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7.0</v>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -534,13 +575,13 @@
       <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="n">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8.0</v>
+      <c r="D8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -548,13 +589,13 @@
       <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="D9" t="n">
-        <v>26.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9.0</v>
+      <c r="D9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
@@ -562,13 +603,13 @@
       <c r="C10" t="s">
         <v>21</v>
       </c>
-      <c r="D10" t="n">
-        <v>32.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10.0</v>
+      <c r="D10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>22</v>
@@ -576,8 +617,280 @@
       <c r="C11" t="s">
         <v>23</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="n">
         <v>41.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD42B306-D4B1-4B26-8DFF-590509F60FCE}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>